<commit_message>
CARTERA VENCIDA. PENDIENTE STACKED PLOT!*
</commit_message>
<xml_diff>
--- a/DATA/CarteraVencida.xlsx
+++ b/DATA/CarteraVencida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lulyelizondo/Documents/tesis/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F65363E-71F6-CF42-9E35-DBB235A3A493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C943029-201F-2A43-8341-5C731954683C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BA89A3CB-3C7B-FF44-8314-39C774EFE286}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" firstSheet="1" activeTab="9" xr2:uid="{BA89A3CB-3C7B-FF44-8314-39C774EFE286}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 cuentas" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm"/>
-    <numFmt numFmtId="174" formatCode="yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -341,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -364,8 +364,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -691,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE29946-AD36-E845-A186-1C4B00D0423C}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -1470,16 +1469,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3CDEB5-C0DF-7E49-98A4-2B8B2DD0F08D}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="14.6640625" style="25" customWidth="1"/>
+    <col min="2" max="5" width="14.6640625" style="24" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1487,16 +1486,16 @@
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F1" s="20" t="s">
@@ -1504,406 +1503,396 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="22">
         <v>44287</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="27">
         <v>1221604.9651668896</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="27">
         <v>77171.151183509995</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="27">
         <v>265854.55207919003</v>
       </c>
-      <c r="E2" s="28">
-        <f>SUM(B2:D2)</f>
+      <c r="E2" s="27">
+        <f t="shared" ref="E2:E18" si="0">SUM(B2:D2)</f>
         <v>1564630.6684295896</v>
       </c>
       <c r="F2" s="21">
-        <f>D2/E2</f>
+        <f t="shared" ref="F2:F18" si="1">D2/E2</f>
         <v>0.16991521222450962</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>44166</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>1203817.4996137901</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="27">
         <v>81132.96965506002</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>244714.08037747006</v>
       </c>
-      <c r="E3" s="28">
-        <f>SUM(B3:D3)</f>
+      <c r="E3" s="27">
+        <f t="shared" si="0"/>
         <v>1529664.5496463201</v>
       </c>
       <c r="F3" s="21">
-        <f>D3/E3</f>
+        <f t="shared" si="1"/>
         <v>0.15997891853743448</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>43800</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="27">
         <v>1225237.7114970102</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="27">
         <v>54169.199341549996</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>169352.71501292003</v>
       </c>
-      <c r="E4" s="28">
-        <f>SUM(B4:D4)</f>
+      <c r="E4" s="27">
+        <f t="shared" si="0"/>
         <v>1448759.6258514803</v>
       </c>
       <c r="F4" s="21">
-        <f>D4/E4</f>
+        <f t="shared" si="1"/>
         <v>0.11689497138863617</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>43435</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>1245911.6393033501</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <v>41058.43927214</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>105528.75429682001</v>
       </c>
-      <c r="E5" s="28">
-        <f>SUM(B5:D5)</f>
+      <c r="E5" s="27">
+        <f t="shared" si="0"/>
         <v>1392498.83287231</v>
       </c>
       <c r="F5" s="21">
-        <f>D5/E5</f>
+        <f t="shared" si="1"/>
         <v>7.5783729081586121E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <v>43070</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <v>1198702.8999999999</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="29">
+      <c r="C6" s="29"/>
+      <c r="D6" s="28">
         <v>102380.04</v>
       </c>
-      <c r="E6" s="28">
-        <f>SUM(B6:D6)</f>
+      <c r="E6" s="27">
+        <f t="shared" si="0"/>
         <v>1301082.94</v>
       </c>
       <c r="F6" s="21">
-        <f>D6/E6</f>
+        <f t="shared" si="1"/>
         <v>7.8688327125402163E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="23">
+      <c r="A7" s="22">
         <v>42705</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>1030076</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>48926</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <v>89731</v>
       </c>
-      <c r="E7" s="28">
-        <f>SUM(B7:D7)</f>
+      <c r="E7" s="27">
+        <f t="shared" si="0"/>
         <v>1168733</v>
       </c>
       <c r="F7" s="21">
-        <f>D7/E7</f>
+        <f t="shared" si="1"/>
         <v>7.6776303912014121E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="23">
+      <c r="A8" s="22">
         <v>42339</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="28">
         <v>940150</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>59067</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>75501</v>
       </c>
-      <c r="E8" s="28">
-        <f>SUM(B8:D8)</f>
+      <c r="E8" s="27">
+        <f t="shared" si="0"/>
         <v>1074718</v>
       </c>
       <c r="F8" s="21">
-        <f>D8/E8</f>
+        <f t="shared" si="1"/>
         <v>7.0251917247129009E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="23">
+      <c r="A9" s="22">
         <v>41974</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="28">
         <v>867072</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <v>55635</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>68351</v>
       </c>
-      <c r="E9" s="28">
-        <f>SUM(B9:D9)</f>
+      <c r="E9" s="27">
+        <f t="shared" si="0"/>
         <v>991058</v>
       </c>
       <c r="F9" s="21">
-        <f>D9/E9</f>
+        <f t="shared" si="1"/>
         <v>6.8967709256168658E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="23">
+      <c r="A10" s="22">
         <v>41609</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="28">
         <v>814897</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="28">
         <v>43739</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>59154</v>
       </c>
-      <c r="E10" s="28">
-        <f>SUM(B10:D10)</f>
+      <c r="E10" s="27">
+        <f t="shared" si="0"/>
         <v>917790</v>
       </c>
       <c r="F10" s="21">
-        <f>D10/E10</f>
+        <f t="shared" si="1"/>
         <v>6.4452652567580815E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="23">
+      <c r="A11" s="22">
         <v>41244</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="28">
         <v>773962</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="28">
         <v>33472</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="28">
         <v>50665</v>
       </c>
-      <c r="E11" s="28">
-        <f>SUM(B11:D11)</f>
+      <c r="E11" s="27">
+        <f t="shared" si="0"/>
         <v>858099</v>
       </c>
       <c r="F11" s="21">
-        <f>D11/E11</f>
+        <f t="shared" si="1"/>
         <v>5.9043303861209484E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="23">
+      <c r="A12" s="22">
         <v>40878</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="27">
         <v>696028</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="27">
         <v>38143</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>49338</v>
       </c>
-      <c r="E12" s="28">
-        <f>SUM(B12:D12)</f>
+      <c r="E12" s="27">
+        <f t="shared" si="0"/>
         <v>783509</v>
       </c>
       <c r="F12" s="21">
-        <f>D12/E12</f>
+        <f t="shared" si="1"/>
         <v>6.2970559368175735E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="23">
+      <c r="A13" s="22">
         <v>40513</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="27">
         <v>637632</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="27">
         <v>28563</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>43216</v>
       </c>
-      <c r="E13" s="28">
-        <f>SUM(B13:D13)</f>
+      <c r="E13" s="27">
+        <f t="shared" si="0"/>
         <v>709411</v>
       </c>
       <c r="F13" s="21">
-        <f>D13/E13</f>
+        <f t="shared" si="1"/>
         <v>6.0918141951562636E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23">
+      <c r="A14" s="22">
         <v>40148</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="27">
         <v>564983</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="27">
         <v>38111</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="27">
         <v>38023</v>
       </c>
-      <c r="E14" s="28">
-        <f>SUM(B14:D14)</f>
+      <c r="E14" s="27">
+        <f t="shared" si="0"/>
         <v>641117</v>
       </c>
       <c r="F14" s="21">
-        <f>D14/E14</f>
+        <f t="shared" si="1"/>
         <v>5.9307427505431928E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="23">
+      <c r="A15" s="22">
         <v>39783</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="27">
         <v>538540</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="27">
         <v>23842</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="27">
         <v>30544</v>
       </c>
-      <c r="E15" s="28">
-        <f>SUM(B15:D15)</f>
+      <c r="E15" s="27">
+        <f t="shared" si="0"/>
         <v>592926</v>
       </c>
       <c r="F15" s="21">
-        <f>D15/E15</f>
+        <f t="shared" si="1"/>
         <v>5.1514016926226883E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="23">
+      <c r="A16" s="22">
         <v>39417</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="27">
         <v>493088</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="27">
         <v>14798</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="27">
         <v>25292</v>
       </c>
-      <c r="E16" s="28">
-        <f>SUM(B16:D16)</f>
+      <c r="E16" s="27">
+        <f t="shared" si="0"/>
         <v>533178</v>
       </c>
       <c r="F16" s="21">
-        <f>D16/E16</f>
+        <f t="shared" si="1"/>
         <v>4.7436315826984612E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="23">
+      <c r="A17" s="22">
         <v>39052</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>427916</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="27">
         <v>21030</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <v>27878</v>
       </c>
-      <c r="E17" s="28">
-        <f>SUM(B17:D17)</f>
+      <c r="E17" s="27">
+        <f t="shared" si="0"/>
         <v>476824</v>
       </c>
       <c r="F17" s="21">
-        <f>D17/E17</f>
+        <f t="shared" si="1"/>
         <v>5.8466016811234332E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="23">
+      <c r="A18" s="22">
         <v>38687</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="27">
         <v>384892</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="27">
         <v>9277</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="27">
         <v>34983</v>
       </c>
-      <c r="E18" s="28">
-        <f>SUM(B18:D18)</f>
+      <c r="E18" s="27">
+        <f t="shared" si="0"/>
         <v>429152</v>
       </c>
       <c r="F18" s="21">
-        <f>D18/E18</f>
+        <f t="shared" si="1"/>
         <v>8.1516572216836919E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="23">
-        <v>38322</v>
-      </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="23">
+      <c r="A19" s="22">
         <v>37956</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B19" s="27">
         <v>312954</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C19" s="27">
         <v>10527</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D19" s="27">
         <v>39518</v>
       </c>
-      <c r="E20" s="31">
-        <f>SUM(B20:D20)</f>
+      <c r="E19" s="30">
+        <f>SUM(B19:D19)</f>
         <v>362999</v>
       </c>
-      <c r="F20" s="21">
-        <f>D20/E20</f>
+      <c r="F19" s="21">
+        <f>D19/E19</f>
         <v>0.10886531367855008</v>
       </c>
     </row>
@@ -7347,7 +7336,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="14.6640625" style="25" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="5" width="14.6640625" style="24" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="14.6640625" style="19" customWidth="1" outlineLevel="1"/>
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -7356,16 +7345,16 @@
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>40</v>
       </c>
       <c r="F1" s="18" t="s">
@@ -7373,19 +7362,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="22">
         <v>44287</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="24">
         <v>4456705</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="24">
         <v>248875</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="24">
         <v>705958</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="24">
         <f>SUM(B2:D2)</f>
         <v>5411538</v>
       </c>
@@ -7395,19 +7384,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>44166</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>4477544</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="24">
         <v>259220</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>664471</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="24">
         <f>SUM(B3:D3)</f>
         <v>5401235</v>
       </c>
@@ -7417,19 +7406,19 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>43800</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>4581746</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>184666</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>463726</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="24">
         <f>SUM(B4:D4)</f>
         <v>5230138</v>
       </c>
@@ -7439,19 +7428,19 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>43435</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>4729523</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>144631</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>290012</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <f>SUM(B5:D5)</f>
         <v>5164166</v>
       </c>
@@ -7461,17 +7450,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <v>43070</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>4741436</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27">
+      <c r="C6" s="25"/>
+      <c r="D6" s="26">
         <v>295745</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <f>SUM(B6:D6)</f>
         <v>5037181</v>
       </c>

</xml_diff>